<commit_message>
Updated port breakout v2.1
</commit_message>
<xml_diff>
--- a/Peripherals/Port Breakout/harp behavior poke port breakout v2.1_BOM.xlsx
+++ b/Peripherals/Port Breakout/harp behavior poke port breakout v2.1_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_behavior\PCB modules\Port Breakout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6990B39-3322-42CF-A089-F976B5F26C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B678742-5956-43F3-8B1F-236FF04CD807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,12 +80,6 @@
     <t>IC2</t>
   </si>
   <si>
-    <t>M74VHC1GT04DTT1G</t>
-  </si>
-  <si>
-    <t>Single inverter buffer</t>
-  </si>
-  <si>
     <t>R1</t>
   </si>
   <si>
@@ -150,6 +144,12 @@
   </si>
   <si>
     <t>DNI</t>
+  </si>
+  <si>
+    <t>M74VHC1GT14DTT1G</t>
+  </si>
+  <si>
+    <t>Single Schmitt-Trigger inverter buffer</t>
   </si>
 </sst>
 </file>
@@ -1082,7 +1082,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,7 +1111,7 @@
         <v>0</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -1127,7 +1127,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -1143,23 +1143,23 @@
         <v>7</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C4" s="7">
         <v>1</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
@@ -1188,90 +1188,90 @@
         <v>1</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C7" s="7">
         <v>1</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8" s="7">
         <v>1</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9" s="7">
         <v>1</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" s="7">
         <v>2</v>
       </c>
       <c r="D10" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>23</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>25</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" s="7">
         <v>1</v>
       </c>
       <c r="D11" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="14" t="s">
         <v>26</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>28</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
@@ -1303,7 +1303,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
@@ -1321,7 +1321,7 @@
         <v>8</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>

</xml_diff>